<commit_message>
Lista se muestra en GUI
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -130,7 +130,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Numero de Lista"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="3" name="2024-11-15 00:56:20"/>
+    <tableColumn id="3" name="2024-11-15 02:23:39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2024-11-15 00:56:20</t>
+          <t>2024-11-15 02:23:39</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Puntual</t>
+          <t>Retardo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Interfaz muestra puntuales y retardos
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -130,7 +130,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Numero de Lista"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="3" name="2024-11-15 12:31:45"/>
+    <tableColumn id="3" name="2024-11-15 12:37:41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2024-11-15 12:31:45</t>
+          <t>2024-11-15 12:37:41</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Puntual</t>
+          <t>Retardo</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Puntual</t>
+          <t>Retardo</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Puntual</t>
+          <t>Retardo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Faltas despues de 2 asistencias y countdown implementado
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -130,7 +130,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Numero de Lista"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="3" name="2024-11-15 12:37:41"/>
+    <tableColumn id="3" name="2024-11-15 16:57:30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2024-11-15 12:37:41</t>
+          <t>2024-11-15 16:57:30</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Falta</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added speech recognition sounds
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -46,7 +46,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -77,12 +77,6 @@
         <bgColor rgb="00B83227"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F3B431"/>
-        <bgColor rgb="00F3B431"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -444,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -533,9 +527,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1002,7 +993,7 @@
       </c>
       <c r="C6" s="19" t="inlineStr">
         <is>
-          <t>15/11/2024 22:43</t>
+          <t>16/11/2024 00:24</t>
         </is>
       </c>
       <c r="D6" s="21" t="inlineStr">
@@ -1169,12 +1160,12 @@
       <c r="O8" s="26" t="n"/>
       <c r="P8" s="26" t="n"/>
       <c r="Q8" s="26" t="n"/>
-      <c r="R8" s="34" t="inlineStr">
+      <c r="R8" s="26" t="n"/>
+      <c r="S8" s="34" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="S8" s="26" t="n"/>
       <c r="T8" s="26" t="n"/>
       <c r="U8" s="26" t="n"/>
       <c r="V8" s="26" t="n"/>
@@ -1214,12 +1205,12 @@
       <c r="O9" s="26" t="n"/>
       <c r="P9" s="26" t="n"/>
       <c r="Q9" s="26" t="n"/>
-      <c r="R9" s="34" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="S9" s="26" t="n"/>
+      <c r="R9" s="26" t="n"/>
+      <c r="S9" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
       <c r="T9" s="26" t="n"/>
       <c r="U9" s="26" t="n"/>
       <c r="V9" s="26" t="n"/>
@@ -1259,12 +1250,12 @@
       <c r="O10" s="26" t="n"/>
       <c r="P10" s="26" t="n"/>
       <c r="Q10" s="26" t="n"/>
-      <c r="R10" s="35" t="inlineStr">
+      <c r="R10" s="26" t="n"/>
+      <c r="S10" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S10" s="26" t="n"/>
       <c r="T10" s="26" t="n"/>
       <c r="U10" s="26" t="n"/>
       <c r="V10" s="26" t="n"/>
@@ -1304,12 +1295,12 @@
       <c r="O11" s="26" t="n"/>
       <c r="P11" s="26" t="n"/>
       <c r="Q11" s="26" t="n"/>
-      <c r="R11" s="35" t="inlineStr">
+      <c r="R11" s="26" t="n"/>
+      <c r="S11" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S11" s="26" t="n"/>
       <c r="T11" s="26" t="n"/>
       <c r="U11" s="26" t="n"/>
       <c r="V11" s="26" t="n"/>
@@ -1349,12 +1340,12 @@
       <c r="O12" s="26" t="n"/>
       <c r="P12" s="26" t="n"/>
       <c r="Q12" s="26" t="n"/>
-      <c r="R12" s="36" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S12" s="26" t="n"/>
+      <c r="R12" s="26" t="n"/>
+      <c r="S12" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
       <c r="T12" s="26" t="n"/>
       <c r="U12" s="26" t="n"/>
       <c r="V12" s="26" t="n"/>
@@ -1394,12 +1385,12 @@
       <c r="O13" s="26" t="n"/>
       <c r="P13" s="26" t="n"/>
       <c r="Q13" s="26" t="n"/>
-      <c r="R13" s="35" t="inlineStr">
+      <c r="R13" s="26" t="n"/>
+      <c r="S13" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S13" s="26" t="n"/>
       <c r="T13" s="26" t="n"/>
       <c r="U13" s="26" t="n"/>
       <c r="V13" s="26" t="n"/>
@@ -1439,12 +1430,12 @@
       <c r="O14" s="26" t="n"/>
       <c r="P14" s="26" t="n"/>
       <c r="Q14" s="26" t="n"/>
-      <c r="R14" s="35" t="inlineStr">
+      <c r="R14" s="26" t="n"/>
+      <c r="S14" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S14" s="26" t="n"/>
       <c r="T14" s="26" t="n"/>
       <c r="U14" s="26" t="n"/>
       <c r="V14" s="26" t="n"/>
@@ -1484,12 +1475,12 @@
       <c r="O15" s="26" t="n"/>
       <c r="P15" s="26" t="n"/>
       <c r="Q15" s="26" t="n"/>
-      <c r="R15" s="36" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S15" s="26" t="n"/>
+      <c r="R15" s="26" t="n"/>
+      <c r="S15" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
       <c r="T15" s="26" t="n"/>
       <c r="U15" s="26" t="n"/>
       <c r="V15" s="26" t="n"/>
@@ -1529,12 +1520,12 @@
       <c r="O16" s="26" t="n"/>
       <c r="P16" s="26" t="n"/>
       <c r="Q16" s="26" t="n"/>
-      <c r="R16" s="35" t="inlineStr">
+      <c r="R16" s="26" t="n"/>
+      <c r="S16" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S16" s="26" t="n"/>
       <c r="T16" s="26" t="n"/>
       <c r="U16" s="26" t="n"/>
       <c r="V16" s="26" t="n"/>
@@ -1574,12 +1565,12 @@
       <c r="O17" s="26" t="n"/>
       <c r="P17" s="26" t="n"/>
       <c r="Q17" s="26" t="n"/>
-      <c r="R17" s="35" t="inlineStr">
+      <c r="R17" s="26" t="n"/>
+      <c r="S17" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S17" s="26" t="n"/>
       <c r="T17" s="26" t="n"/>
       <c r="U17" s="26" t="n"/>
       <c r="V17" s="26" t="n"/>
@@ -1619,12 +1610,12 @@
       <c r="O18" s="26" t="n"/>
       <c r="P18" s="26" t="n"/>
       <c r="Q18" s="26" t="n"/>
-      <c r="R18" s="35" t="inlineStr">
+      <c r="R18" s="26" t="n"/>
+      <c r="S18" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S18" s="26" t="n"/>
       <c r="T18" s="26" t="n"/>
       <c r="U18" s="26" t="n"/>
       <c r="V18" s="26" t="n"/>
@@ -1660,12 +1651,12 @@
       <c r="O19" s="26" t="n"/>
       <c r="P19" s="26" t="n"/>
       <c r="Q19" s="26" t="n"/>
-      <c r="R19" s="35" t="inlineStr">
+      <c r="R19" s="26" t="n"/>
+      <c r="S19" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S19" s="26" t="n"/>
       <c r="T19" s="26" t="n"/>
       <c r="U19" s="26" t="n"/>
       <c r="V19" s="26" t="n"/>
@@ -1701,12 +1692,12 @@
       <c r="O20" s="26" t="n"/>
       <c r="P20" s="26" t="n"/>
       <c r="Q20" s="26" t="n"/>
-      <c r="R20" s="35" t="inlineStr">
+      <c r="R20" s="26" t="n"/>
+      <c r="S20" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S20" s="26" t="n"/>
       <c r="T20" s="26" t="n"/>
       <c r="U20" s="26" t="n"/>
       <c r="V20" s="26" t="n"/>
@@ -1742,12 +1733,12 @@
       <c r="O21" s="26" t="n"/>
       <c r="P21" s="26" t="n"/>
       <c r="Q21" s="26" t="n"/>
-      <c r="R21" s="35" t="inlineStr">
+      <c r="R21" s="26" t="n"/>
+      <c r="S21" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S21" s="26" t="n"/>
       <c r="T21" s="26" t="n"/>
       <c r="U21" s="26" t="n"/>
       <c r="V21" s="26" t="n"/>
@@ -1783,12 +1774,12 @@
       <c r="O22" s="26" t="n"/>
       <c r="P22" s="26" t="n"/>
       <c r="Q22" s="26" t="n"/>
-      <c r="R22" s="35" t="inlineStr">
+      <c r="R22" s="26" t="n"/>
+      <c r="S22" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S22" s="26" t="n"/>
       <c r="T22" s="26" t="n"/>
       <c r="U22" s="26" t="n"/>
       <c r="V22" s="26" t="n"/>
@@ -1824,12 +1815,12 @@
       <c r="O23" s="26" t="n"/>
       <c r="P23" s="26" t="n"/>
       <c r="Q23" s="26" t="n"/>
-      <c r="R23" s="35" t="inlineStr">
+      <c r="R23" s="26" t="n"/>
+      <c r="S23" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S23" s="26" t="n"/>
       <c r="T23" s="26" t="n"/>
       <c r="U23" s="26" t="n"/>
       <c r="V23" s="26" t="n"/>
@@ -1865,12 +1856,12 @@
       <c r="O24" s="26" t="n"/>
       <c r="P24" s="26" t="n"/>
       <c r="Q24" s="26" t="n"/>
-      <c r="R24" s="35" t="inlineStr">
+      <c r="R24" s="26" t="n"/>
+      <c r="S24" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S24" s="26" t="n"/>
       <c r="T24" s="26" t="n"/>
       <c r="U24" s="26" t="n"/>
       <c r="V24" s="26" t="n"/>
@@ -1906,12 +1897,12 @@
       <c r="O25" s="26" t="n"/>
       <c r="P25" s="26" t="n"/>
       <c r="Q25" s="26" t="n"/>
-      <c r="R25" s="35" t="inlineStr">
+      <c r="R25" s="26" t="n"/>
+      <c r="S25" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S25" s="26" t="n"/>
       <c r="T25" s="26" t="n"/>
       <c r="U25" s="26" t="n"/>
       <c r="V25" s="26" t="n"/>
@@ -1947,12 +1938,12 @@
       <c r="O26" s="26" t="n"/>
       <c r="P26" s="26" t="n"/>
       <c r="Q26" s="26" t="n"/>
-      <c r="R26" s="35" t="inlineStr">
+      <c r="R26" s="26" t="n"/>
+      <c r="S26" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S26" s="26" t="n"/>
       <c r="T26" s="26" t="n"/>
       <c r="U26" s="26" t="n"/>
       <c r="V26" s="26" t="n"/>
@@ -1988,12 +1979,12 @@
       <c r="O27" s="26" t="n"/>
       <c r="P27" s="26" t="n"/>
       <c r="Q27" s="26" t="n"/>
-      <c r="R27" s="35" t="inlineStr">
+      <c r="R27" s="26" t="n"/>
+      <c r="S27" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S27" s="26" t="n"/>
       <c r="T27" s="26" t="n"/>
       <c r="U27" s="26" t="n"/>
       <c r="V27" s="26" t="n"/>
@@ -2029,12 +2020,12 @@
       <c r="O28" s="26" t="n"/>
       <c r="P28" s="26" t="n"/>
       <c r="Q28" s="26" t="n"/>
-      <c r="R28" s="35" t="inlineStr">
+      <c r="R28" s="26" t="n"/>
+      <c r="S28" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S28" s="26" t="n"/>
       <c r="T28" s="26" t="n"/>
       <c r="U28" s="26" t="n"/>
       <c r="V28" s="26" t="n"/>
@@ -2070,12 +2061,12 @@
       <c r="O29" s="26" t="n"/>
       <c r="P29" s="26" t="n"/>
       <c r="Q29" s="26" t="n"/>
-      <c r="R29" s="35" t="inlineStr">
+      <c r="R29" s="26" t="n"/>
+      <c r="S29" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S29" s="26" t="n"/>
       <c r="T29" s="26" t="n"/>
       <c r="U29" s="26" t="n"/>
       <c r="V29" s="26" t="n"/>
@@ -2111,12 +2102,12 @@
       <c r="O30" s="26" t="n"/>
       <c r="P30" s="26" t="n"/>
       <c r="Q30" s="26" t="n"/>
-      <c r="R30" s="35" t="inlineStr">
+      <c r="R30" s="26" t="n"/>
+      <c r="S30" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S30" s="26" t="n"/>
       <c r="T30" s="26" t="n"/>
       <c r="U30" s="26" t="n"/>
       <c r="V30" s="26" t="n"/>
@@ -2152,12 +2143,12 @@
       <c r="O31" s="26" t="n"/>
       <c r="P31" s="26" t="n"/>
       <c r="Q31" s="26" t="n"/>
-      <c r="R31" s="35" t="inlineStr">
+      <c r="R31" s="26" t="n"/>
+      <c r="S31" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S31" s="26" t="n"/>
       <c r="T31" s="26" t="n"/>
       <c r="U31" s="26" t="n"/>
       <c r="V31" s="26" t="n"/>
@@ -2193,12 +2184,12 @@
       <c r="O32" s="26" t="n"/>
       <c r="P32" s="26" t="n"/>
       <c r="Q32" s="26" t="n"/>
-      <c r="R32" s="35" t="inlineStr">
+      <c r="R32" s="26" t="n"/>
+      <c r="S32" s="35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S32" s="26" t="n"/>
       <c r="T32" s="26" t="n"/>
       <c r="U32" s="26" t="n"/>
       <c r="V32" s="26" t="n"/>
@@ -2586,94 +2577,94 @@
       <c r="AH42" s="29" t="n"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B43" s="37" t="inlineStr">
+      <c r="B43" s="36" t="inlineStr">
         <is>
           <t>OBSERVACIONES</t>
         </is>
       </c>
-      <c r="C43" s="38" t="n"/>
-      <c r="D43" s="38" t="n"/>
-      <c r="E43" s="38" t="n"/>
-      <c r="F43" s="38" t="n"/>
-      <c r="G43" s="38" t="n"/>
-      <c r="H43" s="38" t="n"/>
-      <c r="I43" s="38" t="n"/>
-      <c r="J43" s="38" t="n"/>
-      <c r="K43" s="38" t="n"/>
-      <c r="L43" s="38" t="n"/>
-      <c r="M43" s="38" t="n"/>
-      <c r="N43" s="38" t="n"/>
-      <c r="O43" s="38" t="n"/>
-      <c r="P43" s="38" t="n"/>
-      <c r="Q43" s="38" t="n"/>
-      <c r="R43" s="38" t="n"/>
-      <c r="S43" s="38" t="n"/>
-      <c r="T43" s="38" t="n"/>
-      <c r="U43" s="38" t="n"/>
-      <c r="V43" s="38" t="n"/>
-      <c r="W43" s="38" t="n"/>
-      <c r="X43" s="38" t="n"/>
-      <c r="Y43" s="38" t="n"/>
-      <c r="Z43" s="38" t="n"/>
-      <c r="AA43" s="38" t="n"/>
-      <c r="AB43" s="38" t="n"/>
-      <c r="AC43" s="38" t="n"/>
-      <c r="AD43" s="38" t="n"/>
-      <c r="AE43" s="38" t="n"/>
-      <c r="AF43" s="38" t="n"/>
-      <c r="AG43" s="38" t="n"/>
-      <c r="AH43" s="39" t="n"/>
+      <c r="C43" s="37" t="n"/>
+      <c r="D43" s="37" t="n"/>
+      <c r="E43" s="37" t="n"/>
+      <c r="F43" s="37" t="n"/>
+      <c r="G43" s="37" t="n"/>
+      <c r="H43" s="37" t="n"/>
+      <c r="I43" s="37" t="n"/>
+      <c r="J43" s="37" t="n"/>
+      <c r="K43" s="37" t="n"/>
+      <c r="L43" s="37" t="n"/>
+      <c r="M43" s="37" t="n"/>
+      <c r="N43" s="37" t="n"/>
+      <c r="O43" s="37" t="n"/>
+      <c r="P43" s="37" t="n"/>
+      <c r="Q43" s="37" t="n"/>
+      <c r="R43" s="37" t="n"/>
+      <c r="S43" s="37" t="n"/>
+      <c r="T43" s="37" t="n"/>
+      <c r="U43" s="37" t="n"/>
+      <c r="V43" s="37" t="n"/>
+      <c r="W43" s="37" t="n"/>
+      <c r="X43" s="37" t="n"/>
+      <c r="Y43" s="37" t="n"/>
+      <c r="Z43" s="37" t="n"/>
+      <c r="AA43" s="37" t="n"/>
+      <c r="AB43" s="37" t="n"/>
+      <c r="AC43" s="37" t="n"/>
+      <c r="AD43" s="37" t="n"/>
+      <c r="AE43" s="37" t="n"/>
+      <c r="AF43" s="37" t="n"/>
+      <c r="AG43" s="37" t="n"/>
+      <c r="AH43" s="38" t="n"/>
     </row>
     <row r="44">
-      <c r="B44" s="40" t="n"/>
-      <c r="AH44" s="41" t="n"/>
+      <c r="B44" s="39" t="n"/>
+      <c r="AH44" s="40" t="n"/>
     </row>
     <row r="45">
-      <c r="B45" s="42" t="n"/>
-      <c r="AH45" s="41" t="n"/>
+      <c r="B45" s="41" t="n"/>
+      <c r="AH45" s="40" t="n"/>
     </row>
     <row r="46">
-      <c r="B46" s="42" t="n"/>
-      <c r="AH46" s="41" t="n"/>
+      <c r="B46" s="41" t="n"/>
+      <c r="AH46" s="40" t="n"/>
     </row>
     <row r="47">
-      <c r="B47" s="42" t="n"/>
-      <c r="AH47" s="41" t="n"/>
+      <c r="B47" s="41" t="n"/>
+      <c r="AH47" s="40" t="n"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B48" s="43" t="n"/>
-      <c r="C48" s="44" t="n"/>
-      <c r="D48" s="44" t="n"/>
-      <c r="E48" s="44" t="n"/>
-      <c r="F48" s="44" t="n"/>
-      <c r="G48" s="44" t="n"/>
-      <c r="H48" s="44" t="n"/>
-      <c r="I48" s="44" t="n"/>
-      <c r="J48" s="44" t="n"/>
-      <c r="K48" s="44" t="n"/>
-      <c r="L48" s="44" t="n"/>
-      <c r="M48" s="44" t="n"/>
-      <c r="N48" s="44" t="n"/>
-      <c r="O48" s="44" t="n"/>
-      <c r="P48" s="44" t="n"/>
-      <c r="Q48" s="44" t="n"/>
-      <c r="R48" s="44" t="n"/>
-      <c r="S48" s="44" t="n"/>
-      <c r="T48" s="44" t="n"/>
-      <c r="U48" s="44" t="n"/>
-      <c r="V48" s="44" t="n"/>
-      <c r="W48" s="44" t="n"/>
-      <c r="X48" s="44" t="n"/>
-      <c r="Y48" s="44" t="n"/>
-      <c r="Z48" s="44" t="n"/>
-      <c r="AA48" s="44" t="n"/>
-      <c r="AB48" s="44" t="n"/>
-      <c r="AC48" s="44" t="n"/>
-      <c r="AD48" s="44" t="n"/>
-      <c r="AE48" s="44" t="n"/>
-      <c r="AF48" s="44" t="n"/>
-      <c r="AG48" s="44" t="n"/>
-      <c r="AH48" s="45" t="n"/>
+      <c r="B48" s="42" t="n"/>
+      <c r="C48" s="43" t="n"/>
+      <c r="D48" s="43" t="n"/>
+      <c r="E48" s="43" t="n"/>
+      <c r="F48" s="43" t="n"/>
+      <c r="G48" s="43" t="n"/>
+      <c r="H48" s="43" t="n"/>
+      <c r="I48" s="43" t="n"/>
+      <c r="J48" s="43" t="n"/>
+      <c r="K48" s="43" t="n"/>
+      <c r="L48" s="43" t="n"/>
+      <c r="M48" s="43" t="n"/>
+      <c r="N48" s="43" t="n"/>
+      <c r="O48" s="43" t="n"/>
+      <c r="P48" s="43" t="n"/>
+      <c r="Q48" s="43" t="n"/>
+      <c r="R48" s="43" t="n"/>
+      <c r="S48" s="43" t="n"/>
+      <c r="T48" s="43" t="n"/>
+      <c r="U48" s="43" t="n"/>
+      <c r="V48" s="43" t="n"/>
+      <c r="W48" s="43" t="n"/>
+      <c r="X48" s="43" t="n"/>
+      <c r="Y48" s="43" t="n"/>
+      <c r="Z48" s="43" t="n"/>
+      <c r="AA48" s="43" t="n"/>
+      <c r="AB48" s="43" t="n"/>
+      <c r="AC48" s="43" t="n"/>
+      <c r="AD48" s="43" t="n"/>
+      <c r="AE48" s="43" t="n"/>
+      <c r="AF48" s="43" t="n"/>
+      <c r="AG48" s="43" t="n"/>
+      <c r="AH48" s="44" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Interfaz mejorada con colores de la escuela
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C6" s="19" t="inlineStr">
         <is>
-          <t>16/11/2024 00:39</t>
+          <t>16/11/2024 17:03</t>
         </is>
       </c>
       <c r="D6" s="21" t="inlineStr">
@@ -1215,9 +1215,9 @@
       <c r="P9" s="26" t="n"/>
       <c r="Q9" s="26" t="n"/>
       <c r="R9" s="26" t="n"/>
-      <c r="S9" s="34" t="inlineStr">
-        <is>
-          <t>P</t>
+      <c r="S9" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
         </is>
       </c>
       <c r="T9" s="26" t="n"/>
@@ -1260,9 +1260,9 @@
       <c r="P10" s="26" t="n"/>
       <c r="Q10" s="26" t="n"/>
       <c r="R10" s="26" t="n"/>
-      <c r="S10" s="34" t="inlineStr">
-        <is>
-          <t>P</t>
+      <c r="S10" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
         </is>
       </c>
       <c r="T10" s="26" t="n"/>
@@ -1440,9 +1440,9 @@
       <c r="P14" s="26" t="n"/>
       <c r="Q14" s="26" t="n"/>
       <c r="R14" s="26" t="n"/>
-      <c r="S14" s="34" t="inlineStr">
-        <is>
-          <t>P</t>
+      <c r="S14" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
         </is>
       </c>
       <c r="T14" s="26" t="n"/>
@@ -1485,9 +1485,9 @@
       <c r="P15" s="26" t="n"/>
       <c r="Q15" s="26" t="n"/>
       <c r="R15" s="26" t="n"/>
-      <c r="S15" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
+      <c r="S15" s="36" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
       <c r="T15" s="26" t="n"/>
@@ -1575,9 +1575,9 @@
       <c r="P17" s="26" t="n"/>
       <c r="Q17" s="26" t="n"/>
       <c r="R17" s="26" t="n"/>
-      <c r="S17" s="36" t="inlineStr">
-        <is>
-          <t>R</t>
+      <c r="S17" s="35" t="inlineStr">
+        <is>
+          <t>F</t>
         </is>
       </c>
       <c r="T17" s="26" t="n"/>
@@ -1620,9 +1620,9 @@
       <c r="P18" s="26" t="n"/>
       <c r="Q18" s="26" t="n"/>
       <c r="R18" s="26" t="n"/>
-      <c r="S18" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
+      <c r="S18" s="36" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
       <c r="T18" s="26" t="n"/>
@@ -1661,11 +1661,7 @@
       <c r="P19" s="26" t="n"/>
       <c r="Q19" s="26" t="n"/>
       <c r="R19" s="26" t="n"/>
-      <c r="S19" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S19" s="26" t="n"/>
       <c r="T19" s="26" t="n"/>
       <c r="U19" s="26" t="n"/>
       <c r="V19" s="26" t="n"/>
@@ -1702,11 +1698,7 @@
       <c r="P20" s="26" t="n"/>
       <c r="Q20" s="26" t="n"/>
       <c r="R20" s="26" t="n"/>
-      <c r="S20" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S20" s="26" t="n"/>
       <c r="T20" s="26" t="n"/>
       <c r="U20" s="26" t="n"/>
       <c r="V20" s="26" t="n"/>
@@ -1743,11 +1735,7 @@
       <c r="P21" s="26" t="n"/>
       <c r="Q21" s="26" t="n"/>
       <c r="R21" s="26" t="n"/>
-      <c r="S21" s="36" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="S21" s="26" t="n"/>
       <c r="T21" s="26" t="n"/>
       <c r="U21" s="26" t="n"/>
       <c r="V21" s="26" t="n"/>
@@ -1784,11 +1772,7 @@
       <c r="P22" s="26" t="n"/>
       <c r="Q22" s="26" t="n"/>
       <c r="R22" s="26" t="n"/>
-      <c r="S22" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S22" s="26" t="n"/>
       <c r="T22" s="26" t="n"/>
       <c r="U22" s="26" t="n"/>
       <c r="V22" s="26" t="n"/>
@@ -1825,11 +1809,7 @@
       <c r="P23" s="26" t="n"/>
       <c r="Q23" s="26" t="n"/>
       <c r="R23" s="26" t="n"/>
-      <c r="S23" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S23" s="26" t="n"/>
       <c r="T23" s="26" t="n"/>
       <c r="U23" s="26" t="n"/>
       <c r="V23" s="26" t="n"/>
@@ -1866,11 +1846,7 @@
       <c r="P24" s="26" t="n"/>
       <c r="Q24" s="26" t="n"/>
       <c r="R24" s="26" t="n"/>
-      <c r="S24" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S24" s="26" t="n"/>
       <c r="T24" s="26" t="n"/>
       <c r="U24" s="26" t="n"/>
       <c r="V24" s="26" t="n"/>
@@ -1907,11 +1883,7 @@
       <c r="P25" s="26" t="n"/>
       <c r="Q25" s="26" t="n"/>
       <c r="R25" s="26" t="n"/>
-      <c r="S25" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S25" s="26" t="n"/>
       <c r="T25" s="26" t="n"/>
       <c r="U25" s="26" t="n"/>
       <c r="V25" s="26" t="n"/>
@@ -1948,11 +1920,7 @@
       <c r="P26" s="26" t="n"/>
       <c r="Q26" s="26" t="n"/>
       <c r="R26" s="26" t="n"/>
-      <c r="S26" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S26" s="26" t="n"/>
       <c r="T26" s="26" t="n"/>
       <c r="U26" s="26" t="n"/>
       <c r="V26" s="26" t="n"/>
@@ -1989,11 +1957,7 @@
       <c r="P27" s="26" t="n"/>
       <c r="Q27" s="26" t="n"/>
       <c r="R27" s="26" t="n"/>
-      <c r="S27" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S27" s="26" t="n"/>
       <c r="T27" s="26" t="n"/>
       <c r="U27" s="26" t="n"/>
       <c r="V27" s="26" t="n"/>
@@ -2030,11 +1994,7 @@
       <c r="P28" s="26" t="n"/>
       <c r="Q28" s="26" t="n"/>
       <c r="R28" s="26" t="n"/>
-      <c r="S28" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S28" s="26" t="n"/>
       <c r="T28" s="26" t="n"/>
       <c r="U28" s="26" t="n"/>
       <c r="V28" s="26" t="n"/>
@@ -2071,11 +2031,7 @@
       <c r="P29" s="26" t="n"/>
       <c r="Q29" s="26" t="n"/>
       <c r="R29" s="26" t="n"/>
-      <c r="S29" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S29" s="26" t="n"/>
       <c r="T29" s="26" t="n"/>
       <c r="U29" s="26" t="n"/>
       <c r="V29" s="26" t="n"/>
@@ -2112,11 +2068,7 @@
       <c r="P30" s="26" t="n"/>
       <c r="Q30" s="26" t="n"/>
       <c r="R30" s="26" t="n"/>
-      <c r="S30" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S30" s="26" t="n"/>
       <c r="T30" s="26" t="n"/>
       <c r="U30" s="26" t="n"/>
       <c r="V30" s="26" t="n"/>
@@ -2153,11 +2105,7 @@
       <c r="P31" s="26" t="n"/>
       <c r="Q31" s="26" t="n"/>
       <c r="R31" s="26" t="n"/>
-      <c r="S31" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S31" s="26" t="n"/>
       <c r="T31" s="26" t="n"/>
       <c r="U31" s="26" t="n"/>
       <c r="V31" s="26" t="n"/>
@@ -2194,11 +2142,7 @@
       <c r="P32" s="26" t="n"/>
       <c r="Q32" s="26" t="n"/>
       <c r="R32" s="26" t="n"/>
-      <c r="S32" s="35" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="S32" s="26" t="n"/>
       <c r="T32" s="26" t="n"/>
       <c r="U32" s="26" t="n"/>
       <c r="V32" s="26" t="n"/>

</xml_diff>